<commit_message>
Oprava data a optimalizace
</commit_message>
<xml_diff>
--- a/data_for_testing/excel_new.xlsx
+++ b/data_for_testing/excel_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserPhD\OneDrive - Univerzita Karlova\spidia ČLÁNEK 2 obnoveno 2022\aplikace_predikce\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserPhD\OneDrive - Univerzita Karlova\spidia ČLÁNEK 2 obnoveno 2022\aplikace_predikce\data_for_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -279,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +297,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,8 +333,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -341,18 +367,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Poznámka" xfId="2" builtinId="10"/>
+    <cellStyle name="Správně" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,808 +2054,808 @@
         <v>12.571833965</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>16.816850495000001</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="4">
         <v>16.028224765000001</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <v>8.7583154650000008</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="4">
         <v>10.624943395000001</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="4">
         <v>7.5638125049999996</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="4">
         <v>8.9127535299999998</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="4">
         <v>14.855291435</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="4">
         <v>15.904966975000001</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="4">
         <v>12.229487904999999</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="4">
         <v>10.649238025000001</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="4">
         <v>14.814367745</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="4">
         <v>12.329444544999999</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="4">
         <v>12.026573454999999</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="4">
         <v>12.764893075</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="4">
         <v>9.3900773710000003</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="4">
         <v>8.9552766049999999</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="4">
         <v>15.265084855</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="4">
         <v>10.171371635</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="4">
         <v>12.759006585</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="4">
         <v>12.361035305</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>17.655638305</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="4">
         <v>16.803730345000002</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="4">
         <v>9.4546920409999995</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="4">
         <v>11.303341144999999</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="4">
         <v>7.9922696340000003</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="4">
         <v>9.4961306620000006</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="4">
         <v>15.251459815</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="4">
         <v>17.551005225000001</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="4">
         <v>12.804142375</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="4">
         <v>12.073334364999999</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="4">
         <v>15.551007765</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="4">
         <v>13.017662655000001</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="4">
         <v>12.602524695</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="4">
         <v>13.598590785000001</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="4">
         <v>9.7595135150000001</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="4">
         <v>9.6937249550000004</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="4">
         <v>16.047843714999999</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="4">
         <v>10.854980615000001</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="4">
         <v>13.304352464999999</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="4">
         <v>14.195050224999999</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>17.396799235</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="4">
         <v>16.303416915</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="4">
         <v>8.9831896600000007</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="4">
         <v>11.038770215</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="4">
         <v>7.7119096559999996</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="4">
         <v>9.2201541959999993</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="4">
         <v>15.590239235</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="4">
         <v>16.697273965000001</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="4">
         <v>12.688044945</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="4">
         <v>11.092201785</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>17.760271585000002</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="4">
         <v>16.447845215000001</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="4">
         <v>9.8027290649999994</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="4">
         <v>11.730714215000001</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="4">
         <v>8.5217396189999999</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="4">
         <v>9.6748169449999999</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="4">
         <v>15.668805225</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="4">
         <v>16.304310274999999</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="4">
         <v>12.884110554999999</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="4">
         <v>11.682083065</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>15.729475754999999</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="4">
         <v>12.777101235</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="4">
         <v>13.474846265</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="4">
         <v>14.055182465</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="4">
         <v>10.262951765</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="4">
         <v>9.636148575</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="4">
         <v>15.920294195</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="4">
         <v>10.637302345</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="4">
         <v>13.137737215</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="4">
         <v>13.373540275</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>17.172157134999999</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="4">
         <v>15.828216955</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="4">
         <v>9.5245418209999997</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="4">
         <v>11.258589215000001</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="4">
         <v>7.8498095059999997</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="4">
         <v>8.5731942589999992</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="4">
         <v>15.070254475</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="4">
         <v>16.196355574999998</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="4">
         <v>12.608941035000001</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="4">
         <v>11.674209885</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>15.968100894999999</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="4">
         <v>17.906238895000001</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="4">
         <v>8.8521794140000001</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="4">
         <v>10.306223425000001</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="4">
         <v>6.6774083739999996</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="4">
         <v>7.8907382310000003</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="4">
         <v>14.389587734999999</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="4">
         <v>15.473260274999999</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="4">
         <v>11.205605155000001</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="4">
         <v>10.770684335</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>15.444842805</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="4">
         <v>17.991501475</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="4">
         <v>7.9652924719999998</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="4">
         <v>9.4377027689999995</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="4">
         <v>6.2091636909999997</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="4">
         <v>7.6308928539999998</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="4">
         <v>13.922727314999999</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="4">
         <v>13.917761705</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="4">
         <v>10.482106914999999</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="4">
         <v>9.9978662150000002</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="4">
         <v>15.751256715</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="4">
         <v>17.347175555</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="4">
         <v>7.6409570789999997</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="4">
         <v>9.1819399530000005</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="4">
         <v>6.5279837980000002</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="4">
         <v>6.4969609330000004</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="4">
         <v>13.403376955000001</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="4">
         <v>15.352516124999999</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="4">
         <v>10.535011285</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="4">
         <v>9.6400807650000004</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>17.833328224999999</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="4">
         <v>18.377691715000001</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="4">
         <v>9.2360239039999996</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="4">
         <v>10.889552184999999</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="4">
         <v>7.6704678990000001</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="4">
         <v>8.4522068059999995</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="4">
         <v>15.144224964999999</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="4">
         <v>16.489160985000002</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="4">
         <v>12.259899935</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="4">
         <v>11.335266975</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>17.225749385</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="4">
         <v>17.061998705000001</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="4">
         <v>9.8310187649999996</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="4">
         <v>11.504013765</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="4">
         <v>8.2652895879999999</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="4">
         <v>9.2814134310000007</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="4">
         <v>15.368534325000001</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="4">
         <v>16.698521974999998</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="4">
         <v>12.356930824999999</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="4">
         <v>11.450165245000001</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="4">
         <v>13.627208175</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="4">
         <v>13.654784715</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="4">
         <v>11.558296224999999</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="4">
         <v>13.693354905</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="4">
         <v>9.0673524430000008</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="4">
         <v>7.5855846570000001</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="4">
         <v>14.136896674999999</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="4">
         <v>9.7804271749999998</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="4">
         <v>11.465038195</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K53" s="4">
         <v>13.322014855000001</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="4">
         <v>13.514497785</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="4">
         <v>15.114174465</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>11.006753775</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="4">
         <v>13.840529015</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="4">
         <v>9.4211794950000005</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="4">
         <v>8.1085195829999996</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="4">
         <v>13.723424465000001</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="4">
         <v>10.168503845</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="4">
         <v>11.340473695</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K54" s="4">
         <v>13.125516155</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="4">
         <v>13.472408065</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="4">
         <v>12.594787295</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>9.6956783150000003</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="4">
         <v>11.779595355</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="4">
         <v>7.9952762850000001</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="4">
         <v>6.2224414530000001</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55" s="4">
         <v>12.652646765</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55" s="4">
         <v>10.026923695000001</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="4">
         <v>10.517438244999999</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K55" s="4">
         <v>11.788902435000001</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="4">
         <v>13.994111315</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="4">
         <v>16.293679635</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>12.817600454999999</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="4">
         <v>14.898285365</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="4">
         <v>10.929236805</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="4">
         <v>7.8204118710000001</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="4">
         <v>14.794415345000001</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="4">
         <v>11.106793014999999</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="4">
         <v>12.159722145</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56" s="4">
         <v>15.006515755000001</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="4">
         <v>14.915766335000001</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="4">
         <v>14.049652455</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="4">
         <v>11.161661595</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="4">
         <v>14.213076655</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="4">
         <v>9.7984912350000002</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="4">
         <v>8.5509264869999999</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57" s="4">
         <v>15.151244865000001</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57" s="4">
         <v>12.191421835</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="4">
         <v>12.679737944999999</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57" s="4">
         <v>12.732208555</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="4">
         <v>15.074752824999999</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="4">
         <v>14.714032745000001</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="4">
         <v>12.551390095</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="4">
         <v>14.941024725</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="4">
         <v>11.028515375</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="4">
         <v>9.3253120329999994</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H58" s="4">
         <v>15.458773335</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58" s="4">
         <v>11.856647345000001</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="4">
         <v>13.083870565</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K58" s="4">
         <v>14.177661205</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="4">
         <v>15.917522294999999</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="4">
         <v>15.403337295</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="4">
         <v>9.9021162349999994</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="4">
         <v>11.518200405</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="4">
         <v>7.7105099819999996</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="4">
         <v>8.1078316909999995</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="4">
         <v>14.800586935</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59" s="4">
         <v>12.441390934999999</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59" s="4">
         <v>11.531157015</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K59" s="4">
         <v>12.153485345</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="4">
         <v>15.049472495</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="4">
         <v>16.003223245000001</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="4">
         <v>9.0126056729999995</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="4">
         <v>10.488572695</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="4">
         <v>7.2320996099999997</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="4">
         <v>7.7950023279999998</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="4">
         <v>13.997431055</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="4">
         <v>12.533103205</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="4">
         <v>10.773826065</v>
       </c>
-      <c r="K60" s="3">
+      <c r="K60" s="4">
         <v>11.639717765</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="4">
         <v>17.590432305</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="4">
         <v>17.580224515000001</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="4">
         <v>11.913874845</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="4">
         <v>12.926428274999999</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="4">
         <v>9.2583309620000005</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="4">
         <v>7.5695342490000002</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H61" s="4">
         <v>14.786433515000001</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="4">
         <v>16.022236525</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="4">
         <v>12.554905335000001</v>
       </c>
-      <c r="K61" s="3">
+      <c r="K61" s="4">
         <v>13.773085585</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="4">
         <v>14.357209675</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="4">
         <v>15.990968685</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="4">
         <v>9.5763196900000001</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="4">
         <v>11.137399925</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62" s="4">
         <v>8.0729735300000005</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="4">
         <v>7.1686406399999996</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H62" s="4">
         <v>13.969878254999999</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62" s="4">
         <v>11.404226625</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="4">
         <v>11.171313245</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K62" s="4">
         <v>11.924473275</v>
       </c>
     </row>

</xml_diff>